<commit_message>
Added Github repo link + demoed + removed file-dependent req.txt
</commit_message>
<xml_diff>
--- a/example_excel_data.xlsx
+++ b/example_excel_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/rachel_estilo_avanade_com/Documents/Townhall/demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/rachel_estilo_avanade_com/Documents/Townhall/streamlit_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_158311114753A6BF6625B4155C05963804FED178" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BD78440-3157-496A-98BB-8F3334F44C4D}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_6D53C27473F4D23DDBBC6E47ECD7F6C32C8C4121" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F397FCBC-CFC2-4F15-8568-179D841DFA97}"/>
   <bookViews>
-    <workbookView xWindow="31860" yWindow="1665" windowWidth="17205" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33930" yWindow="3540" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,18 +43,21 @@
     <t>Total Cost</t>
   </si>
   <si>
+    <t>Southwest</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Pen</t>
+  </si>
+  <si>
     <t>Midwest</t>
   </si>
   <si>
     <t>Pencil</t>
   </si>
   <si>
-    <t>Pen</t>
-  </si>
-  <si>
-    <t>Arthur</t>
-  </si>
-  <si>
     <t>Jardine</t>
   </si>
   <si>
@@ -104,9 +107,6 @@
   </si>
   <si>
     <t>Katie</t>
-  </si>
-  <si>
-    <t>Southwest</t>
   </si>
   <si>
     <t>Southeast</t>
@@ -465,7 +465,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,10 +501,10 @@
         <v>44613</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -524,13 +524,13 @@
         <v>44517</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>11</v>
@@ -547,13 +547,13 @@
         <v>44500</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -570,13 +570,13 @@
         <v>44483</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -593,10 +593,10 @@
         <v>44466</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -616,13 +616,13 @@
         <v>44449</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>7</v>
@@ -639,13 +639,13 @@
         <v>44432</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -662,13 +662,13 @@
         <v>44415</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -685,13 +685,13 @@
         <v>44398</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -708,13 +708,13 @@
         <v>44381</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -731,13 +731,13 @@
         <v>44364</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -754,13 +754,13 @@
         <v>44347</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13">
         <v>9</v>
@@ -777,13 +777,13 @@
         <v>44330</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>22</v>
@@ -800,10 +800,10 @@
         <v>44313</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
@@ -823,13 +823,13 @@
         <v>44296</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E16">
         <v>8</v>
@@ -846,13 +846,13 @@
         <v>44279</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -869,13 +869,13 @@
         <v>44262</v>
       </c>
       <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
         <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
       </c>
       <c r="E18">
         <v>7</v>
@@ -892,13 +892,13 @@
         <v>44245</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -915,13 +915,13 @@
         <v>44228</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E20">
         <v>9</v>
@@ -938,13 +938,13 @@
         <v>44211</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E21">
         <v>12</v>
@@ -961,13 +961,13 @@
         <v>44194</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E22">
         <v>21</v>
@@ -984,13 +984,13 @@
         <v>44177</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E23">
         <v>3</v>
@@ -1007,13 +1007,13 @@
         <v>44160</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E24">
         <v>8</v>
@@ -1030,10 +1030,10 @@
         <v>44143</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1053,10 +1053,10 @@
         <v>44126</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
@@ -1076,13 +1076,13 @@
         <v>44109</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E27">
         <v>28</v>
@@ -1099,13 +1099,13 @@
         <v>44092</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E28">
         <v>16</v>
@@ -1122,13 +1122,13 @@
         <v>44075</v>
       </c>
       <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
         <v>26</v>
       </c>
-      <c r="C29" t="s">
-        <v>25</v>
-      </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -1145,13 +1145,13 @@
         <v>44058</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E30">
         <v>12</v>
@@ -1168,13 +1168,13 @@
         <v>44041</v>
       </c>
       <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
         <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" t="s">
-        <v>12</v>
       </c>
       <c r="E31">
         <v>13</v>
@@ -1191,13 +1191,13 @@
         <v>44024</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E32">
         <v>7</v>
@@ -1214,13 +1214,13 @@
         <v>44007</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D33" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E33">
         <v>7</v>
@@ -1237,13 +1237,13 @@
         <v>43990</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E34">
         <v>6</v>
@@ -1260,13 +1260,13 @@
         <v>43973</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E35">
         <v>5</v>
@@ -1283,13 +1283,13 @@
         <v>43956</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
         <v>11</v>
-      </c>
-      <c r="D36" t="s">
-        <v>8</v>
       </c>
       <c r="E36">
         <v>2</v>
@@ -1306,13 +1306,13 @@
         <v>43939</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -1329,13 +1329,13 @@
         <v>43922</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E38">
         <v>9</v>
@@ -1352,13 +1352,13 @@
         <v>43905</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E39">
         <v>8</v>
@@ -1378,7 +1378,7 @@
         <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
@@ -1398,13 +1398,13 @@
         <v>43870</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
         <v>11</v>
-      </c>
-      <c r="D41" t="s">
-        <v>8</v>
       </c>
       <c r="E41">
         <v>2</v>
@@ -1421,13 +1421,13 @@
         <v>43853</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -1444,13 +1444,13 @@
         <v>43836</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E43">
         <v>12</v>
@@ -1470,6 +1470,6 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{dd1e4005-c2ec-4102-89a4-937c1aac37c3}" enabled="1" method="Privileged" siteId="{cf36141c-ddd7-45a7-b073-111f66d0b30c}" removed="0"/>
+  <clbl:label id="{5fae8262-b78e-4366-8929-a5d6aac95320}" enabled="1" method="Standard" siteId="{cf36141c-ddd7-45a7-b073-111f66d0b30c}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Enabled filling out indiv item price and total price
</commit_message>
<xml_diff>
--- a/example_excel_data.xlsx
+++ b/example_excel_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/rachel_estilo_avanade_com/Documents/Townhall/streamlit_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6D53C27473F4D23DDBBC6E47ECD7F6C32C8C4121" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F397FCBC-CFC2-4F15-8568-179D841DFA97}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_6D53C27473F4D23DDBBC6E47ECD7F6C32C8C4121" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D587744-12B1-4FDB-9BAD-96906442C575}"/>
   <bookViews>
-    <workbookView xWindow="33930" yWindow="3540" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="31">
   <si>
     <t>Order Date</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Southeast</t>
+  </si>
+  <si>
+    <t>Michael</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,967 +501,990 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>44613</v>
+        <v>44680</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>1.5</v>
+        <v>1.29</v>
       </c>
       <c r="G2">
-        <v>18</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>44517</v>
+        <v>44613</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
       <c r="F3">
-        <v>3.99</v>
+        <v>1.5</v>
       </c>
       <c r="G3">
-        <v>43.89</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>44500</v>
+        <v>44517</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
         <v>11</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
       <c r="F4">
-        <v>1.4</v>
+        <v>3.99</v>
       </c>
       <c r="G4">
-        <v>2.8</v>
+        <v>43.89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>44483</v>
+        <v>44500</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>3.99</v>
+        <v>1.4</v>
       </c>
       <c r="G5">
-        <v>11.97</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>44466</v>
+        <v>44483</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>1.5</v>
+        <v>3.99</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>11.97</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>44449</v>
+        <v>44466</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="G7">
-        <v>9.8000000000000007</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>44432</v>
+        <v>44449</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>1.29</v>
+        <v>1.4</v>
       </c>
       <c r="G8">
-        <v>3.87</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>44415</v>
+        <v>44432</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>5.29</v>
+        <v>1.29</v>
       </c>
       <c r="G9">
-        <v>10.58</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>44398</v>
+        <v>44415</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <v>5.29</v>
       </c>
       <c r="G10">
-        <v>5.29</v>
+        <v>10.58</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>44381</v>
+        <v>44398</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>5.29</v>
       </c>
       <c r="G11">
-        <v>15.87</v>
+        <v>5.29</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>44364</v>
+        <v>44381</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>1.29</v>
+        <v>5.29</v>
       </c>
       <c r="G12">
-        <v>6.45</v>
+        <v>15.87</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>44347</v>
+        <v>44364</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>3.99</v>
+        <v>1.29</v>
       </c>
       <c r="G13">
-        <v>35.909999999999997</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>44330</v>
+        <v>44347</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E14">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>1.4</v>
+        <v>3.99</v>
       </c>
       <c r="G14">
-        <v>30.8</v>
+        <v>35.909999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>44313</v>
+        <v>44330</v>
       </c>
       <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
       <c r="F15">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="G15">
-        <v>1.5</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>44296</v>
+        <v>44313</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E16">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="G16">
-        <v>11.2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>44279</v>
+        <v>44296</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F17">
-        <v>5.29</v>
+        <v>1.4</v>
       </c>
       <c r="G17">
-        <v>5.29</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>44262</v>
+        <v>44279</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>3.99</v>
+        <v>5.29</v>
       </c>
       <c r="G18">
-        <v>27.93</v>
+        <v>5.29</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>44245</v>
+        <v>44262</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F19">
         <v>3.99</v>
       </c>
       <c r="G19">
-        <v>15.96</v>
+        <v>27.93</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>44228</v>
+        <v>44245</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E20">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>1.29</v>
+        <v>3.99</v>
       </c>
       <c r="G20">
-        <v>11.61</v>
+        <v>15.96</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>44211</v>
+        <v>44228</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
       <c r="E21">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F21">
         <v>1.29</v>
       </c>
       <c r="G21">
-        <v>15.48</v>
+        <v>11.61</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>44194</v>
+        <v>44211</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E22">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F22">
-        <v>5.29</v>
+        <v>1.29</v>
       </c>
       <c r="G22">
-        <v>11.09</v>
+        <v>15.48</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>44177</v>
+        <v>44194</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F23">
-        <v>1.4</v>
+        <v>5.29</v>
       </c>
       <c r="G23">
-        <v>4.2</v>
+        <v>11.09</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>44160</v>
+        <v>44177</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>5.29</v>
+        <v>1.4</v>
       </c>
       <c r="G24">
-        <v>42.32</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>44143</v>
+        <v>44160</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E25">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F25">
-        <v>1.5</v>
+        <v>5.29</v>
       </c>
       <c r="G25">
-        <v>22.5</v>
+        <v>42.32</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>44126</v>
+        <v>44143</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F26">
         <v>1.5</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>44109</v>
+        <v>44126</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E27">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="F27">
-        <v>3.99</v>
+        <v>1.5</v>
       </c>
       <c r="G27">
-        <v>11.72</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>44092</v>
+        <v>44109</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E28">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F28">
-        <v>5.29</v>
+        <v>3.99</v>
       </c>
       <c r="G28">
-        <v>84.64</v>
+        <v>11.72</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>44075</v>
+        <v>44092</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F29">
-        <v>1.29</v>
+        <v>5.29</v>
       </c>
       <c r="G29">
-        <v>2.58</v>
+        <v>84.64</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>44058</v>
+        <v>44075</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E30">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F30">
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="G30">
-        <v>16.8</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>44041</v>
+        <v>44058</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E31">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31">
-        <v>3.99</v>
+        <v>1.4</v>
       </c>
       <c r="G31">
-        <v>51.87</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>44024</v>
+        <v>44041</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
       </c>
       <c r="E32">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F32">
         <v>3.99</v>
       </c>
       <c r="G32">
-        <v>27.93</v>
+        <v>51.87</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>44007</v>
+        <v>44024</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E33">
         <v>7</v>
       </c>
       <c r="F33">
-        <v>1.4</v>
+        <v>3.99</v>
       </c>
       <c r="G33">
-        <v>9.8000000000000007</v>
+        <v>27.93</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>43990</v>
+        <v>44007</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E34">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F34">
-        <v>3.99</v>
+        <v>1.4</v>
       </c>
       <c r="G34">
-        <v>23.94</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>43973</v>
+        <v>43990</v>
       </c>
       <c r="B35" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E35">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F35">
-        <v>1.4</v>
+        <v>3.99</v>
       </c>
       <c r="G35">
-        <v>7</v>
+        <v>23.94</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>43956</v>
+        <v>43973</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F36">
         <v>1.4</v>
       </c>
       <c r="G36">
-        <v>2.8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>43939</v>
+        <v>43956</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F37">
         <v>1.4</v>
       </c>
       <c r="G37">
-        <v>5.6</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>43922</v>
+        <v>43939</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E38">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>3.99</v>
+        <v>1.4</v>
       </c>
       <c r="G38">
-        <v>35.909999999999997</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>43905</v>
+        <v>43922</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E39">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F39">
-        <v>1.4</v>
+        <v>3.99</v>
       </c>
       <c r="G39">
-        <v>11.2</v>
+        <v>35.909999999999997</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>43887</v>
+        <v>43905</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F40">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="G40">
-        <v>1.5</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>43870</v>
+        <v>43887</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="G41">
-        <v>2.8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>43853</v>
+        <v>43870</v>
       </c>
       <c r="B42" t="s">
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F42">
-        <v>3.99</v>
+        <v>1.4</v>
       </c>
       <c r="G42">
-        <v>19.95</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
+        <v>43853</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>3.99</v>
+      </c>
+      <c r="G43">
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
         <v>43836</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>22</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>23</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>11</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <v>12</v>
       </c>
-      <c r="F43">
+      <c r="F44">
         <v>1.4</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>16.8</v>
       </c>
     </row>

</xml_diff>